<commit_message>
Made changes to a few files
</commit_message>
<xml_diff>
--- a/Test_Framework/_Tests.xlsx
+++ b/Test_Framework/_Tests.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8042FE49-0001-4D86-8ED7-873181532A60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="11743" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="15">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -56,12 +57,24 @@
   </si>
   <si>
     <t>Framework\InitAllApplications.xaml</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>AppEx: Object reference not set to an instance of an object. at Source: Invoke ACME_OpenAndLogin workflow</t>
+  </si>
+  <si>
+    <t>AppEx: Could not find file 'C:\Users\smit.rathore\Documents\UiPath\WI4-Performer-Demo-Can\Test_Framework\Test_ProcessTransaction.xaml'. at Source: mscorlib</t>
+  </si>
+  <si>
+    <t>AppEx: Cannot find the UI element corresponding to this selector: &lt;html title='ACME System 1*' /&gt; at Source: Invoke ACME_LogoutAndClose workflow: Attach Browser 'iexplore.exe ACME'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -390,19 +403,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="41.88671875" customWidth="1"/>
+    <col min="1" max="2" width="41.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="20.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -410,7 +423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -418,7 +431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -426,7 +439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -434,7 +447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -442,7 +455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -450,7 +463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -458,7 +471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -466,7 +479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -474,7 +487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -482,7 +495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -490,7 +503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -498,7 +511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -506,7 +519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -514,7 +527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -522,7 +535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -530,7 +543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -538,7 +551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -546,7 +559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -554,7 +567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -564,7 +577,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Success,BRE,AppEx"</formula1>
     </dataValidation>
   </dataValidations>
@@ -574,22 +587,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="46.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="135.5546875" customWidth="1"/>
+    <col min="1" max="1" width="46.3046875" customWidth="1"/>
+    <col min="2" max="2" width="12.3046875" customWidth="1"/>
+    <col min="3" max="3" width="11.4609375" customWidth="1"/>
+    <col min="4" max="4" width="135.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -603,7 +616,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -614,7 +627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -622,10 +635,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -636,7 +652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -647,7 +663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -658,7 +674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -669,7 +685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -677,10 +693,13 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -688,10 +707,13 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -699,10 +721,13 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -710,10 +735,13 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -721,10 +749,13 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -732,10 +763,13 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -743,10 +777,13 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -754,10 +791,13 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -765,10 +805,13 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -776,10 +819,13 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -787,10 +833,13 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -801,7 +850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -813,9 +862,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B28" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Success,BRE,AppEx"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>